<commit_message>
prettified excel output and added paces per run
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +61,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,59 +442,67 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Week</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Monday</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Friday</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Total miles</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -493,7 +511,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -503,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -513,25 +531,21 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>5 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+          <t>8 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -540,7 +554,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -550,7 +564,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -560,25 +574,21 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>5 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+          <t>10 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -587,7 +597,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -597,7 +607,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -607,25 +617,21 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+          <t>6 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" s="3" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -634,7 +640,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -644,7 +650,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -654,25 +660,21 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+          <t>10 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -681,7 +683,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -691,7 +693,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -701,25 +703,21 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+          <t>12 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" s="3" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -728,7 +726,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -738,7 +736,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -748,25 +746,21 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+          <t>14 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -775,7 +769,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -785,7 +779,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -795,25 +789,21 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+          <t>10 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -822,7 +812,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -832,7 +822,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>7 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -842,25 +832,21 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+          <t>14 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -869,7 +855,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -879,7 +865,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>7 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -889,25 +875,21 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>16 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -916,7 +898,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -926,7 +908,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>7 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -936,25 +918,21 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+          <t>18 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A12" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -963,7 +941,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -973,7 +951,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -983,25 +961,21 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+          <t>10 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A13" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1010,7 +984,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>5 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1020,7 +994,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1030,25 +1004,21 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>10 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+          <t>14 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="A14" s="3" t="n">
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1057,7 +1027,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>5 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1067,7 +1037,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1077,25 +1047,21 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>10 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+          <t>16 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="A15" s="3" t="n">
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1104,7 +1070,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>5 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1114,7 +1080,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1124,25 +1090,21 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>10 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+          <t>18 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A16" s="3" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1151,7 +1113,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1161,7 +1123,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1171,25 +1133,21 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+          <t>10 @ 8:30-9:30 min/mile</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="A17" s="3" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1198,7 +1156,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 @ 7:15 min/mile</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1208,7 +1166,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1218,18 +1176,16 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 @ 8:00 min/mile</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+          <t>26 @ 8:00 min/mile</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>